<commit_message>
Did another trial of the homework.  Added more calculations to the homework #04 spreadsheet.
</commit_message>
<xml_diff>
--- a/Gradiance Submissions/Homework #04/CS256 - Homework #04 - Problem Calculations.xlsx
+++ b/Gradiance Submissions/Homework #04/CS256 - Homework #04 - Problem Calculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="22">
   <si>
     <t>SSE</t>
   </si>
@@ -303,6 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -312,7 +313,6 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA101"/>
+  <dimension ref="A1:AI102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,12 +628,12 @@
     <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -652,8 +652,14 @@
       <c r="H2" s="13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>4</v>
       </c>
@@ -672,8 +678,14 @@
       <c r="H3" s="11">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J3" s="11">
+        <v>0</v>
+      </c>
+      <c r="K3" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>9</v>
       </c>
@@ -692,8 +704,14 @@
       <c r="H4" s="11">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J4" s="11">
+        <v>6</v>
+      </c>
+      <c r="K4" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -712,8 +730,14 @@
       <c r="H5" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J5" s="11">
+        <v>3</v>
+      </c>
+      <c r="K5" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -723,8 +747,11 @@
       <c r="G7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>(A3+A4+A5)/3</f>
         <v>5</v>
@@ -749,8 +776,16 @@
         <f>(H3+H4+H5)/3</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f>(J3+J4+J5)/3</f>
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <f>(K3+K4+K5)/3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>($A$8-A3)^2+($B$8-B3)^2</f>
         <v>10</v>
@@ -763,8 +798,12 @@
         <f>(G$8-G3)^2+(H$8-H3)^2</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f>(J$8-J3)^2+(K$8-K3)^2</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A12" si="0">($A$8-A4)^2+($B$8-B4)^2</f>
         <v>16</v>
@@ -777,8 +816,12 @@
         <f>(G$8-G4)^2+(H$8-H4)^2</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f>(J$8-J4)^2+(K$8-K4)^2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -791,8 +834,12 @@
         <f>(G$8-G5)^2+(H$8-H5)^2</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f>(J$8-J5)^2+(K$8-K5)^2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>SUM(A10:A12)</f>
         <v>44</v>
@@ -805,9 +852,13 @@
         <f>SUM(G10:G12)</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" s="1">
+        <f>SUM(J10:J12)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -817,8 +868,11 @@
       <c r="O16" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -858,8 +912,21 @@
         <f>(O18-O17)^2+(P18-P17)^2</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V17">
+        <v>10</v>
+      </c>
+      <c r="W17">
+        <v>4</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z17">
+        <f>(V18-V17)^2+(W18-W17)^2</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -899,8 +966,21 @@
         <f>(O17-O19)^2+(P17-P19)^2</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V18">
+        <v>4</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z18">
+        <f>(V17-V19)^2+(W17-W19)^2</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -940,8 +1020,21 @@
         <f>(O19-O18)^2+(P19-P18)^2</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V19">
+        <v>7</v>
+      </c>
+      <c r="W19">
+        <v>7</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z19">
+        <f>(V19-V18)^2+(W19-W18)^2</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -963,8 +1056,15 @@
         <f>CONCATENATE("Closest Points: ", IF(MIN(S$17:S$19)=S$17,R$17,IF(MIN(S$17:S$19)=S$18,R$18,R19)))</f>
         <v>Closest Points: (1,3)</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="str">
+        <f>CONCATENATE("Closest Points: ", IF(MIN(Z$17:Z$19)=Z$17,Y$17,IF(MIN(Z$17:Z$19)=Z$18,Y$18,Y19)))</f>
+        <v>Closest Points: (1,3)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>(A17+A18+A19)/3</f>
         <v>3</v>
@@ -1013,8 +1113,24 @@
         <f>IF(MIN(S$17:S$19)=S$17,AVERAGE(P$17:P$18),IF(MIN(S$17:S$19)=S$18,AVERAGE(P$17,P$19),AVERAGE(P$18:P$19)))</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V22">
+        <f>(V17+V18+V19)/3</f>
+        <v>7</v>
+      </c>
+      <c r="W22">
+        <f>(W17+W18+W19)/3</f>
+        <v>4</v>
+      </c>
+      <c r="Y22">
+        <f>IF(MIN(Z$17:Z$19)=Z$17,AVERAGE(V$17:V$18),IF(MIN(Z$17:Z$19)=Z$18,AVERAGE(V17,V19),AVERAGE(V18:V19)))</f>
+        <v>8.5</v>
+      </c>
+      <c r="Z22">
+        <f>IF(MIN(Z$17:Z$19)=Z$17,AVERAGE(W$17:W$18),IF(MIN(Z$17:Z$19)=Z$18,AVERAGE(W$17,W$19),AVERAGE(W$18:W$19)))</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>6</v>
       </c>
@@ -1045,8 +1161,18 @@
       </c>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>IF(OR(MIN(E$17:E$19)=E$17,MIN(E$17:E$19)=E$18),(D$22-A17)^2+(E$22-B17)^2,0)</f>
         <v>8.5</v>
@@ -1071,8 +1197,16 @@
         <f>(O17-AVERAGE(O$17:O$19))^2+(P17-AVERAGE(P$17:P$19))^2</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V24">
+        <f>IF(OR(MIN(Z$17:Z$19)=Z$17,MIN(Z$17:Z$19)=Z$18),(Y$22-V17)^2+(Z$22-W17)^2,0)</f>
+        <v>4.5</v>
+      </c>
+      <c r="Y24">
+        <f>(V17-AVERAGE(V$17:V$19))^2+(W17-AVERAGE(W$17:W$19))^2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>IF(OR(MIN(E$17:E$19)=E$17,MIN(E$17:E$19)=E$19),(D$22-A18)^2+(E$22-B18)^2,0)</f>
         <v>0</v>
@@ -1097,8 +1231,16 @@
         <f t="shared" ref="R25:R26" si="3">(O18-AVERAGE(O$17:O$19))^2+(P18-AVERAGE(P$17:P$19))^2</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V25">
+        <f>IF(OR(MIN(Z$17:Z$19)=Z$17,MIN(Z$17:Z$19)=Z$19),(Y$22-V18)^2+(Z$22-W18)^2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" ref="Y25:Y26" si="4">(V18-AVERAGE(V$17:V$19))^2+(W18-AVERAGE(W$17:W$19))^2</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>IF(OR(MIN(E$17:E$19)=E$18,MIN(E$17:E$19)=E$19),(D$22-A19)^2+(E$22-B19)^2,0)</f>
         <v>8.5</v>
@@ -1123,8 +1265,16 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V26">
+        <f>IF(OR(MIN(Z$17:Z$19)=Z$18,MIN(Z$17:Z$19)=Z$19),(Y$22-V19)^2+(Z$22-W19)^2,0)</f>
+        <v>4.5</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>SUM(A24:A26)</f>
         <v>17</v>
@@ -1149,8 +1299,16 @@
         <f>SUM(R24:R26)</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V27" s="1">
+        <f>SUM(V24:V26)</f>
+        <v>9</v>
+      </c>
+      <c r="Y27">
+        <f>SUM(Y24:Y26)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1172,9 +1330,16 @@
         <f>R27-O27</f>
         <v>19.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V29" t="s">
+        <v>8</v>
+      </c>
+      <c r="W29" s="4">
+        <f>Y27-V27</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1404,7 +1569,7 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>25</v>
       </c>
@@ -1424,7 +1589,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>AVERAGE($A$32:$G$32)</f>
         <v>19.714285714285715</v>
@@ -1443,7 +1608,7 @@
       </c>
       <c r="E50" s="6"/>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>36</v>
       </c>
@@ -1463,7 +1628,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <f>AVERAGE($A$32:$G$32)</f>
         <v>19.714285714285715</v>
@@ -1482,7 +1647,7 @@
       </c>
       <c r="E53" s="6"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>36</v>
       </c>
@@ -1502,7 +1667,7 @@
         <v>Solution</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>AVERAGE($A$32:$H$32)</f>
         <v>25.25</v>
@@ -1521,8 +1686,8 @@
       </c>
       <c r="E56" s="6"/>
     </row>
-    <row r="58" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>18</v>
       </c>
@@ -1586,9 +1751,27 @@
       <c r="AA60">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="AC60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD60">
+        <v>5</v>
+      </c>
+      <c r="AE60">
+        <v>10</v>
+      </c>
+      <c r="AG60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH60">
+        <v>5</v>
+      </c>
+      <c r="AI60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B61">
@@ -1597,7 +1780,7 @@
       <c r="C61">
         <v>5</v>
       </c>
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="16" t="s">
         <v>19</v>
       </c>
       <c r="F61">
@@ -1606,7 +1789,7 @@
       <c r="G61">
         <v>5</v>
       </c>
-      <c r="I61" s="19" t="s">
+      <c r="I61" s="16" t="s">
         <v>19</v>
       </c>
       <c r="J61">
@@ -1615,7 +1798,7 @@
       <c r="K61">
         <v>5</v>
       </c>
-      <c r="M61" s="19" t="s">
+      <c r="M61" s="16" t="s">
         <v>19</v>
       </c>
       <c r="N61">
@@ -1624,7 +1807,7 @@
       <c r="O61">
         <v>5</v>
       </c>
-      <c r="Q61" s="19" t="s">
+      <c r="Q61" s="16" t="s">
         <v>19</v>
       </c>
       <c r="R61">
@@ -1633,7 +1816,7 @@
       <c r="S61">
         <v>5</v>
       </c>
-      <c r="U61" s="19" t="s">
+      <c r="U61" s="16" t="s">
         <v>19</v>
       </c>
       <c r="V61">
@@ -1642,7 +1825,7 @@
       <c r="W61">
         <v>5</v>
       </c>
-      <c r="Y61" s="19" t="s">
+      <c r="Y61" s="16" t="s">
         <v>19</v>
       </c>
       <c r="Z61">
@@ -1651,8 +1834,26 @@
       <c r="AA61">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC61" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD61">
+        <v>20</v>
+      </c>
+      <c r="AE61">
+        <v>5</v>
+      </c>
+      <c r="AG61" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH61">
+        <v>20</v>
+      </c>
+      <c r="AI61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -1674,23 +1875,29 @@
       <c r="Y63" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC63" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C64" t="str">
         <f>IF(((A64-B$60)^2+(B64-C$60)^2) &lt; ((A64-B$61)^2+(B64-C$61)^2), "YELLOW","BLUE")</f>
         <v>YELLOW</v>
       </c>
       <c r="E64">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F64">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G64" t="str">
         <f>IF(((E64-F$60)^2+(F64-G$60)^2) &lt; ((E64-F$61)^2+(F64-G$61)^2), "YELLOW","BLUE")</f>
@@ -1700,7 +1907,7 @@
         <v>6</v>
       </c>
       <c r="J64">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="K64" t="str">
         <f>IF(((I64-J$60)^2+(J64-K$60)^2) &lt; ((I64-J$61)^2+(J64-K$61)^2), "YELLOW","BLUE")</f>
@@ -1710,7 +1917,7 @@
         <v>7</v>
       </c>
       <c r="N64">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O64" t="str">
         <f>IF(((M64-N$60)^2+(N64-O$60)^2) &lt; ((M64-N$61)^2+(N64-O$61)^2), "YELLOW","BLUE")</f>
@@ -1720,7 +1927,7 @@
         <v>6</v>
       </c>
       <c r="R64">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="S64" t="str">
         <f>IF(((Q64-R$60)^2+(R64-S$60)^2) &lt; ((Q64-R$61)^2+(R64-S$61)^2), "YELLOW","BLUE")</f>
@@ -1730,96 +1937,136 @@
         <v>7</v>
       </c>
       <c r="V64">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="W64" t="str">
         <f>IF(((U64-V$60)^2+(V64-W$60)^2) &lt; ((U64-V$61)^2+(V64-W$61)^2), "YELLOW","BLUE")</f>
         <v>YELLOW</v>
       </c>
       <c r="Y64">
+        <v>6</v>
+      </c>
+      <c r="Z64">
         <v>7</v>
-      </c>
-      <c r="Z64">
-        <v>12</v>
       </c>
       <c r="AA64" t="str">
         <f>IF(((Y64-Z$60)^2+(Z64-AA$60)^2) &lt; ((Y64-Z$61)^2+(Z64-AA$61)^2), "YELLOW","BLUE")</f>
         <v>YELLOW</v>
       </c>
-    </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC64">
+        <v>7</v>
+      </c>
+      <c r="AD64">
+        <v>8</v>
+      </c>
+      <c r="AE64" t="str">
+        <f>IF(((AC64-AD$60)^2+(AD64-AE$60)^2) &lt; ((AC64-AD$61)^2+(AD64-AE$61)^2), "YELLOW","BLUE")</f>
+        <v>YELLOW</v>
+      </c>
+      <c r="AG64">
+        <v>7</v>
+      </c>
+      <c r="AH64">
+        <v>12</v>
+      </c>
+      <c r="AI64" t="str">
+        <f>IF(((AG64-AH$60)^2+(AH64-AI$60)^2) &lt; ((AG64-AH$61)^2+(AH64-AI$61)^2), "YELLOW","BLUE")</f>
+        <v>YELLOW</v>
+      </c>
+    </row>
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C65" t="str">
         <f>IF(((A65-B$60)^2+(B65-C$60)^2) &lt; ((A65-B$61)^2+(B65-C$61)^2), "YELLOW","BLUE")</f>
         <v>YELLOW</v>
       </c>
       <c r="E65">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F65">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" t="str">
         <f>IF(((E65-F$60)^2+(F65-G$60)^2) &lt; ((E65-F$61)^2+(F65-G$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="I65">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J65">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K65" t="str">
         <f>IF(((I65-J$60)^2+(J65-K$60)^2) &lt; ((I65-J$61)^2+(J65-K$61)^2), "YELLOW","BLUE")</f>
-        <v>BLUE</v>
+        <v>YELLOW</v>
       </c>
       <c r="M65">
         <v>12</v>
       </c>
       <c r="N65">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O65" t="str">
         <f>IF(((M65-N$60)^2+(N65-O$60)^2) &lt; ((M65-N$61)^2+(N65-O$61)^2), "YELLOW","BLUE")</f>
-        <v>YELLOW</v>
+        <v>BLUE</v>
       </c>
       <c r="Q65">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="R65">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S65" t="str">
         <f>IF(((Q65-R$60)^2+(R65-S$60)^2) &lt; ((Q65-R$61)^2+(R65-S$61)^2), "YELLOW","BLUE")</f>
-        <v>YELLOW</v>
+        <v>BLUE</v>
       </c>
       <c r="U65">
         <v>12</v>
       </c>
       <c r="V65">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="W65" t="str">
         <f>IF(((U65-V$60)^2+(V65-W$60)^2) &lt; ((U65-V$61)^2+(V65-W$61)^2), "YELLOW","BLUE")</f>
-        <v>BLUE</v>
+        <v>YELLOW</v>
       </c>
       <c r="Y65">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z65">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AA65" t="str">
         <f>IF(((Y65-Z$60)^2+(Z65-AA$60)^2) &lt; ((Y65-Z$61)^2+(Z65-AA$61)^2), "YELLOW","BLUE")</f>
         <v>YELLOW</v>
       </c>
-    </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC65">
+        <v>12</v>
+      </c>
+      <c r="AD65">
+        <v>5</v>
+      </c>
+      <c r="AE65" t="str">
+        <f>IF(((AC65-AD$60)^2+(AD65-AE$60)^2) &lt; ((AC65-AD$61)^2+(AD65-AE$61)^2), "YELLOW","BLUE")</f>
+        <v>BLUE</v>
+      </c>
+      <c r="AG65">
+        <v>12</v>
+      </c>
+      <c r="AH65">
+        <v>8</v>
+      </c>
+      <c r="AI65" t="str">
+        <f>IF(((AG65-AH$60)^2+(AH65-AI$60)^2) &lt; ((AG65-AH$61)^2+(AH65-AI$61)^2), "YELLOW","BLUE")</f>
+        <v>YELLOW</v>
+      </c>
+    </row>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>21</v>
       </c>
@@ -1841,1147 +2088,1231 @@
       <c r="Y66" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC66" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C67" t="str">
         <f>IF(((A67-B$60)^2+(B67-C$60)^2) &lt; ((A67-B$61)^2+(B67-C$61)^2), "YELLOW","BLUE")</f>
-        <v>YELLOW</v>
+        <v>BLUE</v>
       </c>
       <c r="E67">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F67">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G67" t="str">
         <f>IF(((E67-F$60)^2+(F67-G$60)^2) &lt; ((E67-F$61)^2+(F67-G$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="I67">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J67">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="K67" t="str">
         <f>IF(((I67-J$60)^2+(J67-K$60)^2) &lt; ((I67-J$61)^2+(J67-K$61)^2), "YELLOW","BLUE")</f>
         <v>YELLOW</v>
       </c>
       <c r="M67">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N67">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O67" t="str">
         <f>IF(((M67-N$60)^2+(N67-O$60)^2) &lt; ((M67-N$61)^2+(N67-O$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="Q67">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="R67">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="S67" t="str">
         <f>IF(((Q67-R$60)^2+(R67-S$60)^2) &lt; ((Q67-R$61)^2+(R67-S$61)^2), "YELLOW","BLUE")</f>
-        <v>BLUE</v>
+        <v>YELLOW</v>
       </c>
       <c r="U67">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="V67">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="W67" t="str">
         <f>IF(((U67-V$60)^2+(V67-W$60)^2) &lt; ((U67-V$61)^2+(V67-W$61)^2), "YELLOW","BLUE")</f>
-        <v>YELLOW</v>
+        <v>BLUE</v>
       </c>
       <c r="Y67">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Z67">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA67" t="str">
         <f>IF(((Y67-Z$60)^2+(Z67-AA$60)^2) &lt; ((Y67-Z$61)^2+(Z67-AA$61)^2), "YELLOW","BLUE")</f>
+        <v>BLUE</v>
+      </c>
+      <c r="AC67">
+        <v>13</v>
+      </c>
+      <c r="AD67">
+        <v>10</v>
+      </c>
+      <c r="AE67" t="str">
+        <f>IF(((AC67-AD$60)^2+(AD67-AE$60)^2) &lt; ((AC67-AD$61)^2+(AD67-AE$61)^2), "YELLOW","BLUE")</f>
         <v>YELLOW</v>
       </c>
-    </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AG67">
+        <v>16</v>
+      </c>
+      <c r="AH67">
+        <v>19</v>
+      </c>
+      <c r="AI67" t="str">
+        <f>IF(((AG67-AH$60)^2+(AH67-AI$60)^2) &lt; ((AG67-AH$61)^2+(AH67-AI$61)^2), "YELLOW","BLUE")</f>
+        <v>YELLOW</v>
+      </c>
+    </row>
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C68" t="str">
         <f>IF(((A68-B$60)^2+(B68-C$60)^2) &lt; ((A68-B$61)^2+(B68-C$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="E68">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F68">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G68" t="str">
         <f>IF(((E68-F$60)^2+(F68-G$60)^2) &lt; ((E68-F$61)^2+(F68-G$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="I68">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="J68">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K68" t="str">
         <f>IF(((I68-J$60)^2+(J68-K$60)^2) &lt; ((I68-J$61)^2+(J68-K$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="M68">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N68">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O68" t="str">
         <f>IF(((M68-N$60)^2+(N68-O$60)^2) &lt; ((M68-N$61)^2+(N68-O$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="Q68">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="R68">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="S68" t="str">
         <f>IF(((Q68-R$60)^2+(R68-S$60)^2) &lt; ((Q68-R$61)^2+(R68-S$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="U68">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="V68">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W68" t="str">
         <f>IF(((U68-V$60)^2+(V68-W$60)^2) &lt; ((U68-V$61)^2+(V68-W$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
       <c r="Y68">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Z68">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="AA68" t="str">
         <f>IF(((Y68-Z$60)^2+(Z68-AA$60)^2) &lt; ((Y68-Z$61)^2+(Z68-AA$61)^2), "YELLOW","BLUE")</f>
         <v>BLUE</v>
       </c>
-    </row>
-    <row r="70" spans="1:27" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="1:27" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E71" s="16" t="s">
+      <c r="AC68">
+        <v>16</v>
+      </c>
+      <c r="AD68">
+        <v>4</v>
+      </c>
+      <c r="AE68" t="str">
+        <f>IF(((AC68-AD$60)^2+(AD68-AE$60)^2) &lt; ((AC68-AD$61)^2+(AD68-AE$61)^2), "YELLOW","BLUE")</f>
+        <v>BLUE</v>
+      </c>
+      <c r="AG68">
+        <v>25</v>
+      </c>
+      <c r="AH68">
+        <v>12</v>
+      </c>
+      <c r="AI68" t="str">
+        <f>IF(((AG68-AH$60)^2+(AH68-AI$60)^2) &lt; ((AG68-AH$61)^2+(AH68-AI$61)^2), "YELLOW","BLUE")</f>
+        <v>BLUE</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="8" t="str">
+        <f>IF(AND(C64="YELLOW",C65="YELLOW",C67="BLUE",C68="BLUE"),"SOLUTION","")</f>
+        <v>SOLUTION</v>
+      </c>
+      <c r="G69" s="8" t="str">
+        <f>IF(AND(G64="YELLOW",G65="YELLOW",G67="BLUE",G68="BLUE"),"SOLUTION","")</f>
+        <v/>
+      </c>
+      <c r="K69" s="8" t="str">
+        <f>IF(AND(K64="YELLOW",K65="YELLOW",K67="BLUE",K68="BLUE"),"SOLUTION","")</f>
+        <v/>
+      </c>
+      <c r="O69" s="8" t="str">
+        <f>IF(AND(O64="YELLOW",O65="YELLOW",O67="BLUE",O68="BLUE"),"SOLUTION","")</f>
+        <v/>
+      </c>
+      <c r="S69" s="8" t="str">
+        <f>IF(AND(S64="YELLOW",S65="YELLOW",S67="BLUE",S68="BLUE"),"SOLUTION","")</f>
+        <v/>
+      </c>
+      <c r="W69" s="8" t="str">
+        <f>IF(AND(W64="YELLOW",W65="YELLOW",W67="BLUE",W68="BLUE"),"SOLUTION","")</f>
+        <v>SOLUTION</v>
+      </c>
+      <c r="AA69" s="8" t="str">
+        <f>IF(AND(AA64="YELLOW",AA65="YELLOW",AA67="BLUE",AA68="BLUE"),"SOLUTION","")</f>
+        <v>SOLUTION</v>
+      </c>
+      <c r="AE69" s="8" t="str">
+        <f>IF(AND(AD64="YELLOW",AD65="YELLOW",AD67="BLUE",AD68="BLUE"),"SOLUTION","")</f>
+        <v/>
+      </c>
+      <c r="AI69" s="8" t="str">
+        <f>IF(AND(AH64="YELLOW",AH65="YELLOW",AH67="BLUE",AH68="BLUE"),"SOLUTION","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:35" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:35" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E72" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F71" s="17"/>
-      <c r="G71" s="18"/>
-      <c r="I71" s="16" t="s">
+      <c r="F72" s="18"/>
+      <c r="G72" s="19"/>
+      <c r="I72" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J71" s="17"/>
-      <c r="K71" s="18"/>
-      <c r="M71" s="16" t="s">
+      <c r="J72" s="18"/>
+      <c r="K72" s="19"/>
+      <c r="M72" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N71" s="17"/>
-      <c r="O71" s="18"/>
-    </row>
-    <row r="72" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E72" t="s">
+      <c r="N72" s="18"/>
+      <c r="O72" s="19"/>
+    </row>
+    <row r="73" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
         <v>12</v>
       </c>
-      <c r="F72">
-        <f>B77</f>
-        <v>4</v>
-      </c>
-      <c r="G72">
-        <f>C77</f>
-        <v>4</v>
-      </c>
-      <c r="I72" t="s">
+      <c r="F73">
+        <f>B78</f>
+        <v>4</v>
+      </c>
+      <c r="G73">
+        <f>C78</f>
+        <v>4</v>
+      </c>
+      <c r="I73" t="s">
         <v>12</v>
       </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
-      <c r="K72">
-        <v>4</v>
-      </c>
-      <c r="M72" t="s">
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>4</v>
+      </c>
+      <c r="M73" t="s">
         <v>12</v>
       </c>
-      <c r="N72">
-        <v>2</v>
-      </c>
-      <c r="O72">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
+      <c r="N73">
+        <v>2</v>
+      </c>
+      <c r="O73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
         <v>13</v>
       </c>
-      <c r="F73">
-        <f>B81</f>
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <f>C81</f>
-        <v>0</v>
-      </c>
-      <c r="I73" t="s">
+      <c r="F74">
+        <f>B82</f>
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <f>C82</f>
+        <v>0</v>
+      </c>
+      <c r="I74" t="s">
         <v>13</v>
       </c>
-      <c r="J73">
-        <v>2</v>
-      </c>
-      <c r="K73">
-        <v>4</v>
-      </c>
-      <c r="M73" t="s">
+      <c r="J74">
+        <v>2</v>
+      </c>
+      <c r="K74">
+        <v>4</v>
+      </c>
+      <c r="M74" t="s">
         <v>13</v>
       </c>
-      <c r="N73">
-        <v>0</v>
-      </c>
-      <c r="O73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A74" s="13" t="s">
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B75" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C75" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E74" s="13" t="s">
+      <c r="E75" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F74" s="14" t="s">
+      <c r="F75" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G74" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I74" s="13" t="s">
+      <c r="G75" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I75" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J74" s="14" t="s">
+      <c r="J75" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K74" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M74" s="13" t="s">
+      <c r="K75" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M75" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N74" s="14" t="s">
+      <c r="N75" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O74" s="14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A75" s="12">
-        <v>1</v>
-      </c>
-      <c r="B75" s="11">
-        <v>0</v>
-      </c>
-      <c r="C75" s="11">
-        <v>4</v>
-      </c>
-      <c r="E75" s="12">
-        <v>1</v>
-      </c>
-      <c r="F75" s="11">
-        <f>MIN((($B$75-F72)^2+($C$75-G72)^2),(($B$75-F73)^2+($C$75-G73)^2))</f>
+      <c r="O75" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A76" s="12">
+        <v>1</v>
+      </c>
+      <c r="B76" s="11">
+        <v>0</v>
+      </c>
+      <c r="C76" s="11">
+        <v>4</v>
+      </c>
+      <c r="E76" s="12">
+        <v>1</v>
+      </c>
+      <c r="F76" s="11">
+        <f>MIN((($B$76-F73)^2+($C$76-G73)^2),(($B$76-F74)^2+($C$76-G74)^2))</f>
         <v>16</v>
       </c>
-      <c r="G75" s="11">
-        <f>IF((($B$75-F72)^2+($C$75-G72)^2)&lt;(($B$75-F73)^2+($C$75-G73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="I75" s="12">
-        <v>1</v>
-      </c>
-      <c r="J75" s="11">
-        <f>MIN((($B$75-J72)^2+($C$75-K72)^2),(($B$75-J73)^2+($C$75-K73)^2))</f>
-        <v>0</v>
-      </c>
-      <c r="K75" s="11">
-        <f>IF((($B$75-J72)^2+($C$75-K72)^2)&lt;(($B$75-J73)^2+($C$75-K73)^2),1,2)</f>
-        <v>1</v>
-      </c>
-      <c r="M75" s="12">
-        <v>1</v>
-      </c>
-      <c r="N75" s="11">
-        <f>MIN((($B$75-N72)^2+($C$75-O72)^2),(($B$75-N73)^2+($C$75-O73)^2))</f>
-        <v>4</v>
-      </c>
-      <c r="O75" s="11">
-        <f>IF((($B$75-N72)^2+($C$75-O72)^2)&lt;(($B$75-N73)^2+($C$75-O73)^2),1,2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A76" s="12">
-        <v>2</v>
-      </c>
-      <c r="B76" s="11">
-        <v>2</v>
-      </c>
-      <c r="C76" s="11">
-        <v>4</v>
-      </c>
-      <c r="E76" s="12">
-        <v>2</v>
-      </c>
-      <c r="F76" s="11">
-        <f>MIN((($B$76-F72)^2+($C$76-G72)^2),(($B$76-F73)^2+($C$76-G73)^2))</f>
-        <v>4</v>
-      </c>
       <c r="G76" s="11">
-        <f>IF((($B$76-F72)^2+($C$76-G72)^2)&lt;(($B$76-F73)^2+($C$76-G73)^2),1,2)</f>
-        <v>1</v>
+        <f>IF((($B$76-F73)^2+($C$76-G73)^2)&lt;(($B$76-F74)^2+($C$76-G74)^2),1,2)</f>
+        <v>2</v>
       </c>
       <c r="I76" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J76" s="11">
-        <f>MIN((($B$76-J72)^2+($C$76-K72)^2),(($B$76-J73)^2+($C$76-K73)^2))</f>
+        <f>MIN((($B$76-J73)^2+($C$76-K73)^2),(($B$76-J74)^2+($C$76-K74)^2))</f>
         <v>0</v>
       </c>
       <c r="K76" s="11">
-        <f>IF((($B$76-J72)^2+($C$76-K72)^2)&lt;(($B$76-J73)^2+($C$76-K73)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$76-J73)^2+($C$76-K73)^2)&lt;(($B$76-J74)^2+($C$76-K74)^2),1,2)</f>
+        <v>1</v>
       </c>
       <c r="M76" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N76" s="11">
-        <f>MIN((($B$76-N72)^2+($C$76-O72)^2),(($B$76-N73)^2+($C$76-O73)^2))</f>
-        <v>0</v>
+        <f>MIN((($B$76-N73)^2+($C$76-O73)^2),(($B$76-N74)^2+($C$76-O74)^2))</f>
+        <v>4</v>
       </c>
       <c r="O76" s="11">
-        <f>IF((($B$76-N72)^2+($C$76-O72)^2)&lt;(($B$76-N73)^2+($C$76-O73)^2),1,2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+        <f>IF((($B$76-N73)^2+($C$76-O73)^2)&lt;(($B$76-N74)^2+($C$76-O74)^2),1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
+        <v>2</v>
+      </c>
+      <c r="B77" s="11">
+        <v>2</v>
+      </c>
+      <c r="C77" s="11">
+        <v>4</v>
+      </c>
+      <c r="E77" s="12">
+        <v>2</v>
+      </c>
+      <c r="F77" s="11">
+        <f>MIN((($B$77-F73)^2+($C$77-G73)^2),(($B$77-F74)^2+($C$77-G74)^2))</f>
+        <v>4</v>
+      </c>
+      <c r="G77" s="11">
+        <f>IF((($B$77-F73)^2+($C$77-G73)^2)&lt;(($B$77-F74)^2+($C$77-G74)^2),1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="I77" s="12">
+        <v>2</v>
+      </c>
+      <c r="J77" s="11">
+        <f>MIN((($B$77-J73)^2+($C$77-K73)^2),(($B$77-J74)^2+($C$77-K74)^2))</f>
+        <v>0</v>
+      </c>
+      <c r="K77" s="11">
+        <f>IF((($B$77-J73)^2+($C$77-K73)^2)&lt;(($B$77-J74)^2+($C$77-K74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="M77" s="12">
+        <v>2</v>
+      </c>
+      <c r="N77" s="11">
+        <f>MIN((($B$77-N73)^2+($C$77-O73)^2),(($B$77-N74)^2+($C$77-O74)^2))</f>
+        <v>0</v>
+      </c>
+      <c r="O77" s="11">
+        <f>IF((($B$77-N73)^2+($C$77-O73)^2)&lt;(($B$77-N74)^2+($C$77-O74)^2),1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A78" s="12">
         <v>3</v>
       </c>
-      <c r="B77" s="11">
-        <v>4</v>
-      </c>
-      <c r="C77" s="11">
-        <v>4</v>
-      </c>
-      <c r="E77" s="12">
+      <c r="B78" s="11">
+        <v>4</v>
+      </c>
+      <c r="C78" s="11">
+        <v>4</v>
+      </c>
+      <c r="E78" s="12">
         <v>3</v>
       </c>
-      <c r="F77" s="11">
-        <f>MIN((($B$77-F72)^2+($C$77-G72)^2),(($B$77-F73)^2+($C$77-G73)^2))</f>
-        <v>0</v>
-      </c>
-      <c r="G77" s="11">
-        <f>IF((($B$77-F72)^2+($C$77-G72)^2)&lt;(($B$77-F73)^2+($C$77-G73)^2),1,2)</f>
-        <v>1</v>
-      </c>
-      <c r="I77" s="12">
+      <c r="F78" s="11">
+        <f>MIN((($B$78-F73)^2+($C$78-G73)^2),(($B$78-F74)^2+($C$78-G74)^2))</f>
+        <v>0</v>
+      </c>
+      <c r="G78" s="11">
+        <f>IF((($B$78-F73)^2+($C$78-G73)^2)&lt;(($B$78-F74)^2+($C$78-G74)^2),1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="I78" s="12">
         <v>3</v>
       </c>
-      <c r="J77" s="11">
-        <f>MIN((($B$77-J72)^2+($C$77-K72)^2),(($B$77-J73)^2+($C$77-K73)^2))</f>
-        <v>4</v>
-      </c>
-      <c r="K77" s="11">
-        <f>IF((($B$77-J72)^2+($C$77-K72)^2)&lt;(($B$77-J73)^2+($C$77-K73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="M77" s="12">
+      <c r="J78" s="11">
+        <f>MIN((($B$78-J73)^2+($C$78-K73)^2),(($B$78-J74)^2+($C$78-K74)^2))</f>
+        <v>4</v>
+      </c>
+      <c r="K78" s="11">
+        <f>IF((($B$78-J73)^2+($C$78-K73)^2)&lt;(($B$78-J74)^2+($C$78-K74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="M78" s="12">
         <v>3</v>
       </c>
-      <c r="N77" s="11">
-        <f>MIN((($B$77-N72)^2+($C$77-O72)^2),(($B$77-N73)^2+($C$77-O73)^2))</f>
-        <v>4</v>
-      </c>
-      <c r="O77" s="11">
-        <f>IF((($B$77-N72)^2+($C$77-O72)^2)&lt;(($B$77-N73)^2+($C$77-O73)^2),1,2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A78" s="12">
-        <v>4</v>
-      </c>
-      <c r="B78" s="11">
-        <v>0</v>
-      </c>
-      <c r="C78" s="11">
-        <v>2</v>
-      </c>
-      <c r="E78" s="12">
-        <v>4</v>
-      </c>
-      <c r="F78" s="11">
-        <f>MIN((($B$78-F72)^2+($C$78-G72)^2),(($B$78-F73)^2+($C$78-G73)^2))</f>
-        <v>4</v>
-      </c>
-      <c r="G78" s="11">
-        <f>IF((($B$78-F72)^2+($C$78-G72)^2)&lt;(($B$78-F73)^2+($C$78-G73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="I78" s="12">
-        <v>4</v>
-      </c>
-      <c r="J78" s="11">
-        <f>MIN((($B$78-J72)^2+($C$78-K72)^2),(($B$78-J73)^2+($C$78-K73)^2))</f>
-        <v>4</v>
-      </c>
-      <c r="K78" s="11">
-        <f>IF((($B$78-J72)^2+($C$78-K72)^2)&lt;(($B$78-J73)^2+($C$78-K73)^2),1,2)</f>
-        <v>1</v>
-      </c>
-      <c r="M78" s="12">
-        <v>4</v>
-      </c>
       <c r="N78" s="11">
-        <f>MIN((($B$78-N72)^2+($C$78-O72)^2),(($B$78-N73)^2+($C$78-O73)^2))</f>
+        <f>MIN((($B$78-N73)^2+($C$78-O73)^2),(($B$78-N74)^2+($C$78-O74)^2))</f>
         <v>4</v>
       </c>
       <c r="O78" s="11">
-        <f>IF((($B$78-N72)^2+($C$78-O72)^2)&lt;(($B$78-N73)^2+($C$78-O73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+        <f>IF((($B$78-N73)^2+($C$78-O73)^2)&lt;(($B$78-N74)^2+($C$78-O74)^2),1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B79" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C79" s="11">
         <v>2</v>
       </c>
       <c r="E79" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" s="11">
-        <f>MIN((($B$79-F72)^2+($C$79-G72)^2),(($B$79-F73)^2+($C$79-G73)^2))</f>
+        <f>MIN((($B$79-F73)^2+($C$79-G73)^2),(($B$79-F74)^2+($C$79-G74)^2))</f>
+        <v>4</v>
+      </c>
+      <c r="G79" s="11">
+        <f>IF((($B$79-F73)^2+($C$79-G73)^2)&lt;(($B$79-F74)^2+($C$79-G74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="I79" s="12">
+        <v>4</v>
+      </c>
+      <c r="J79" s="11">
+        <f>MIN((($B$79-J73)^2+($C$79-K73)^2),(($B$79-J74)^2+($C$79-K74)^2))</f>
+        <v>4</v>
+      </c>
+      <c r="K79" s="11">
+        <f>IF((($B$79-J73)^2+($C$79-K73)^2)&lt;(($B$79-J74)^2+($C$79-K74)^2),1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="M79" s="12">
+        <v>4</v>
+      </c>
+      <c r="N79" s="11">
+        <f>MIN((($B$79-N73)^2+($C$79-O73)^2),(($B$79-N74)^2+($C$79-O74)^2))</f>
+        <v>4</v>
+      </c>
+      <c r="O79" s="11">
+        <f>IF((($B$79-N73)^2+($C$79-O73)^2)&lt;(($B$79-N74)^2+($C$79-O74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A80" s="12">
+        <v>5</v>
+      </c>
+      <c r="B80" s="11">
+        <v>2</v>
+      </c>
+      <c r="C80" s="11">
+        <v>2</v>
+      </c>
+      <c r="E80" s="12">
+        <v>5</v>
+      </c>
+      <c r="F80" s="11">
+        <f>MIN((($B$80-F73)^2+($C$80-G73)^2),(($B$80-F74)^2+($C$80-G74)^2))</f>
         <v>8</v>
       </c>
-      <c r="G79" s="11">
-        <f>IF((($B$79-F72)^2+($C$79-G72)^2)&lt;(($B$79-F73)^2+($C$79-G73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="I79" s="12">
-        <v>5</v>
-      </c>
-      <c r="J79" s="11">
-        <f>MIN((($B$79-J72)^2+($C$79-K72)^2),(($B$79-J73)^2+($C$79-K73)^2))</f>
-        <v>4</v>
-      </c>
-      <c r="K79" s="11">
-        <f>IF((($B$79-J72)^2+($C$79-K72)^2)&lt;(($B$79-J73)^2+($C$79-K73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="M79" s="12">
-        <v>5</v>
-      </c>
-      <c r="N79" s="11">
-        <f>MIN((($B$79-N72)^2+($C$79-O72)^2),(($B$79-N73)^2+($C$79-O73)^2))</f>
-        <v>4</v>
-      </c>
-      <c r="O79" s="11">
-        <f>IF((($B$79-N72)^2+($C$79-O72)^2)&lt;(($B$79-N73)^2+($C$79-O73)^2),1,2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A80" s="12">
-        <v>6</v>
-      </c>
-      <c r="B80" s="11">
-        <v>4</v>
-      </c>
-      <c r="C80" s="11">
-        <v>2</v>
-      </c>
-      <c r="E80" s="12">
-        <v>6</v>
-      </c>
-      <c r="F80" s="11">
-        <f>MIN((($B$80-F72)^2+($C$80-G72)^2),(($B$80-F73)^2+($C$80-G73)^2))</f>
-        <v>4</v>
-      </c>
       <c r="G80" s="11">
-        <f>IF((($B$80-F72)^2+($C$80-G72)^2)&lt;(($B$80-F73)^2+($C$80-G73)^2),1,2)</f>
-        <v>1</v>
+        <f>IF((($B$80-F73)^2+($C$80-G73)^2)&lt;(($B$80-F74)^2+($C$80-G74)^2),1,2)</f>
+        <v>2</v>
       </c>
       <c r="I80" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J80" s="11">
-        <f>MIN((($B$80-J72)^2+($C$80-K72)^2),(($B$80-J73)^2+($C$80-K73)^2))</f>
-        <v>8</v>
+        <f>MIN((($B$80-J73)^2+($C$80-K73)^2),(($B$80-J74)^2+($C$80-K74)^2))</f>
+        <v>4</v>
       </c>
       <c r="K80" s="11">
-        <f>IF((($B$80-J72)^2+($C$80-K72)^2)&lt;(($B$80-J73)^2+($C$80-K73)^2),1,2)</f>
+        <f>IF((($B$80-J73)^2+($C$80-K73)^2)&lt;(($B$80-J74)^2+($C$80-K74)^2),1,2)</f>
         <v>2</v>
       </c>
       <c r="M80" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N80" s="11">
-        <f>MIN((($B$80-N72)^2+($C$80-O72)^2),(($B$80-N73)^2+($C$80-O73)^2))</f>
-        <v>8</v>
+        <f>MIN((($B$80-N73)^2+($C$80-O73)^2),(($B$80-N74)^2+($C$80-O74)^2))</f>
+        <v>4</v>
       </c>
       <c r="O80" s="11">
-        <f>IF((($B$80-N72)^2+($C$80-O72)^2)&lt;(($B$80-N73)^2+($C$80-O73)^2),1,2)</f>
+        <f>IF((($B$80-N73)^2+($C$80-O73)^2)&lt;(($B$80-N74)^2+($C$80-O74)^2),1,2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B81" s="11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C81" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E81" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" s="11">
-        <f>MIN((($B$81-F72)^2+($C$81-G72)^2),(($B$81-F73)^2+($C$81-G73)^2))</f>
-        <v>0</v>
+        <f>MIN((($B$81-F73)^2+($C$81-G73)^2),(($B$81-F74)^2+($C$81-G74)^2))</f>
+        <v>4</v>
       </c>
       <c r="G81" s="11">
-        <f>IF((($B$81-F72)^2+($C$81-G72)^2)&lt;(($B$81-F73)^2+($C$81-G73)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$81-F73)^2+($C$81-G73)^2)&lt;(($B$81-F74)^2+($C$81-G74)^2),1,2)</f>
+        <v>1</v>
       </c>
       <c r="I81" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J81" s="11">
-        <f>MIN((($B$81-J72)^2+($C$81-K72)^2),(($B$81-J73)^2+($C$81-K73)^2))</f>
-        <v>16</v>
+        <f>MIN((($B$81-J73)^2+($C$81-K73)^2),(($B$81-J74)^2+($C$81-K74)^2))</f>
+        <v>8</v>
       </c>
       <c r="K81" s="11">
-        <f>IF((($B$81-J72)^2+($C$81-K72)^2)&lt;(($B$81-J73)^2+($C$81-K73)^2),1,2)</f>
-        <v>1</v>
+        <f>IF((($B$81-J73)^2+($C$81-K73)^2)&lt;(($B$81-J74)^2+($C$81-K74)^2),1,2)</f>
+        <v>2</v>
       </c>
       <c r="M81" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N81" s="11">
-        <f>MIN((($B$81-N72)^2+($C$81-O72)^2),(($B$81-N73)^2+($C$81-O73)^2))</f>
-        <v>0</v>
+        <f>MIN((($B$81-N73)^2+($C$81-O73)^2),(($B$81-N74)^2+($C$81-O74)^2))</f>
+        <v>8</v>
       </c>
       <c r="O81" s="11">
-        <f>IF((($B$81-N72)^2+($C$81-O72)^2)&lt;(($B$81-N73)^2+($C$81-O73)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$81-N73)^2+($C$81-O73)^2)&lt;(($B$81-N74)^2+($C$81-O74)^2),1,2)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B82" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C82" s="11">
         <v>0</v>
       </c>
       <c r="E82" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" s="11">
-        <f>MIN((($B$82-F72)^2+($C$82-G72)^2),(($B$82-F73)^2+($C$82-G73)^2))</f>
-        <v>4</v>
+        <f>MIN((($B$82-F73)^2+($C$82-G73)^2),(($B$82-F74)^2+($C$82-G74)^2))</f>
+        <v>0</v>
       </c>
       <c r="G82" s="11">
-        <f>IF((($B$82-F72)^2+($C$82-G72)^2)&lt;(($B$82-F73)^2+($C$82-G73)^2),1,2)</f>
+        <f>IF((($B$82-F73)^2+($C$82-G73)^2)&lt;(($B$82-F74)^2+($C$82-G74)^2),1,2)</f>
         <v>2</v>
       </c>
       <c r="I82" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J82" s="11">
-        <f>MIN((($B$82-J72)^2+($C$82-K72)^2),(($B$82-J73)^2+($C$82-K73)^2))</f>
+        <f>MIN((($B$82-J73)^2+($C$82-K73)^2),(($B$82-J74)^2+($C$82-K74)^2))</f>
         <v>16</v>
       </c>
       <c r="K82" s="11">
-        <f>IF((($B$82-J72)^2+($C$82-K72)^2)&lt;(($B$82-J73)^2+($C$82-K73)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$82-J73)^2+($C$82-K73)^2)&lt;(($B$82-J74)^2+($C$82-K74)^2),1,2)</f>
+        <v>1</v>
       </c>
       <c r="M82" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N82" s="11">
-        <f>MIN((($B$82-N72)^2+($C$82-O72)^2),(($B$82-N73)^2+($C$82-O73)^2))</f>
-        <v>4</v>
+        <f>MIN((($B$82-N73)^2+($C$82-O73)^2),(($B$82-N74)^2+($C$82-O74)^2))</f>
+        <v>0</v>
       </c>
       <c r="O82" s="11">
-        <f>IF((($B$82-N72)^2+($C$82-O72)^2)&lt;(($B$82-N73)^2+($C$82-O73)^2),1,2)</f>
+        <f>IF((($B$82-N73)^2+($C$82-O73)^2)&lt;(($B$82-N74)^2+($C$82-O74)^2),1,2)</f>
         <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
+        <v>8</v>
+      </c>
+      <c r="B83" s="11">
+        <v>2</v>
+      </c>
+      <c r="C83" s="11">
+        <v>0</v>
+      </c>
+      <c r="E83" s="12">
+        <v>8</v>
+      </c>
+      <c r="F83" s="11">
+        <f>MIN((($B$83-F73)^2+($C$83-G73)^2),(($B$83-F74)^2+($C$83-G74)^2))</f>
+        <v>4</v>
+      </c>
+      <c r="G83" s="11">
+        <f>IF((($B$83-F73)^2+($C$83-G73)^2)&lt;(($B$83-F74)^2+($C$83-G74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="I83" s="12">
+        <v>8</v>
+      </c>
+      <c r="J83" s="11">
+        <f>MIN((($B$83-J73)^2+($C$83-K73)^2),(($B$83-J74)^2+($C$83-K74)^2))</f>
+        <v>16</v>
+      </c>
+      <c r="K83" s="11">
+        <f>IF((($B$83-J73)^2+($C$83-K73)^2)&lt;(($B$83-J74)^2+($C$83-K74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="M83" s="12">
+        <v>8</v>
+      </c>
+      <c r="N83" s="11">
+        <f>MIN((($B$83-N73)^2+($C$83-O73)^2),(($B$83-N74)^2+($C$83-O74)^2))</f>
+        <v>4</v>
+      </c>
+      <c r="O83" s="11">
+        <f>IF((($B$83-N73)^2+($C$83-O73)^2)&lt;(($B$83-N74)^2+($C$83-O74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" s="12">
         <v>9</v>
       </c>
-      <c r="B83" s="11">
-        <v>4</v>
-      </c>
-      <c r="C83" s="11">
-        <v>0</v>
-      </c>
-      <c r="E83" s="12">
+      <c r="B84" s="11">
+        <v>4</v>
+      </c>
+      <c r="C84" s="11">
+        <v>0</v>
+      </c>
+      <c r="E84" s="12">
         <v>9</v>
       </c>
-      <c r="F83" s="11">
-        <f>MIN((($B$83-F72)^2+($C$83-G72)^2),(($B$83-F73)^2+($C$83-G73)^2))</f>
+      <c r="F84" s="11">
+        <f>MIN((($B$84-F73)^2+($C$84-G73)^2),(($B$84-F74)^2+($C$84-G74)^2))</f>
         <v>16</v>
       </c>
-      <c r="G83" s="11">
-        <f>IF((($B$83-F72)^2+($C$83-G72)^2)&lt;(($B$83-F73)^2+($C$83-G73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="I83" s="12">
+      <c r="G84" s="11">
+        <f>IF((($B$84-F73)^2+($C$84-G73)^2)&lt;(($B$84-F74)^2+($C$84-G74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="I84" s="12">
         <v>9</v>
       </c>
-      <c r="J83" s="11">
-        <f>MIN((($B$83-J72)^2+($C$83-K72)^2),(($B$83-J73)^2+($C$83-K73)^2))</f>
+      <c r="J84" s="11">
+        <f>MIN((($B$84-J73)^2+($C$84-K73)^2),(($B$84-J74)^2+($C$84-K74)^2))</f>
         <v>20</v>
       </c>
-      <c r="K83" s="11">
-        <f>IF((($B$83-J72)^2+($C$83-K72)^2)&lt;(($B$83-J73)^2+($C$83-K73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="M83" s="12">
+      <c r="K84" s="11">
+        <f>IF((($B$84-J73)^2+($C$84-K73)^2)&lt;(($B$84-J74)^2+($C$84-K74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="M84" s="12">
         <v>9</v>
       </c>
-      <c r="N83" s="11">
-        <f>MIN((($B$83-N72)^2+($C$83-O72)^2),(($B$83-N73)^2+($C$83-O73)^2))</f>
+      <c r="N84" s="11">
+        <f>MIN((($B$84-N73)^2+($C$84-O73)^2),(($B$84-N74)^2+($C$84-O74)^2))</f>
         <v>16</v>
       </c>
-      <c r="O83" s="11">
-        <f>IF((($B$83-N72)^2+($C$83-O72)^2)&lt;(($B$83-N73)^2+($C$83-O73)^2),1,2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E85" t="s">
-        <v>0</v>
-      </c>
-      <c r="F85" s="15">
-        <f>SUM(F75:F83)</f>
+      <c r="O84" s="11">
+        <f>IF((($B$84-N73)^2+($C$84-O73)^2)&lt;(($B$84-N74)^2+($C$84-O74)^2),1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>0</v>
+      </c>
+      <c r="F86" s="15">
+        <f>SUM(F76:F84)</f>
         <v>56</v>
       </c>
-      <c r="I85" t="s">
-        <v>0</v>
-      </c>
-      <c r="J85" s="15">
-        <f>SUM(J75:J83)</f>
+      <c r="I86" t="s">
+        <v>0</v>
+      </c>
+      <c r="J86" s="15">
+        <f>SUM(J76:J84)</f>
         <v>72</v>
       </c>
-      <c r="M85" t="s">
-        <v>0</v>
-      </c>
-      <c r="N85" s="15">
-        <f>SUM(N75:N83)</f>
+      <c r="M86" t="s">
+        <v>0</v>
+      </c>
+      <c r="N86" s="15">
+        <f>SUM(N76:N84)</f>
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:15" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E87" s="16" t="s">
+    <row r="87" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="1:15" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E88" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F87" s="17"/>
-      <c r="G87" s="18"/>
-      <c r="I87" s="16" t="s">
+      <c r="F88" s="18"/>
+      <c r="G88" s="19"/>
+      <c r="I88" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J87" s="17"/>
-      <c r="K87" s="18"/>
-      <c r="M87" s="16" t="s">
+      <c r="J88" s="18"/>
+      <c r="K88" s="19"/>
+      <c r="M88" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="N87" s="17"/>
-      <c r="O87" s="18"/>
-    </row>
-    <row r="88" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E88" t="s">
+      <c r="N88" s="18"/>
+      <c r="O88" s="19"/>
+    </row>
+    <row r="89" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
         <v>12</v>
       </c>
-      <c r="F88">
-        <f>AVERAGE(B76,B77,B80)</f>
+      <c r="F89">
+        <f>AVERAGE(B77,B78,B81)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="G88">
-        <f>AVERAGE(C76,C77,C80)</f>
+      <c r="G89">
+        <f>AVERAGE(C77,C78,C81)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="I88" t="s">
+      <c r="I89" t="s">
         <v>12</v>
       </c>
-      <c r="J88">
-        <v>0</v>
-      </c>
-      <c r="K88">
-        <v>2</v>
-      </c>
-      <c r="M88" t="s">
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>2</v>
+      </c>
+      <c r="M89" t="s">
         <v>12</v>
       </c>
-      <c r="N88">
-        <f>AVERAGE(B75,B76,B77,B79,B80)</f>
+      <c r="N89">
+        <f>AVERAGE(B76,B77,B78,B80,B81)</f>
         <v>2.4</v>
       </c>
-      <c r="O88">
-        <f>AVERAGE(C75,C76,C77,C79,C80)</f>
+      <c r="O89">
+        <f>AVERAGE(C76,C77,C78,C80,C81)</f>
         <v>3.2</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E89" t="s">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
         <v>13</v>
       </c>
-      <c r="F89">
-        <f>AVERAGE(B75,B78,B79,B81,B82,B83)</f>
+      <c r="F90">
+        <f>AVERAGE(B76,B79,B80,B82,B83,B84)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G89">
-        <f>AVERAGE(C75,C78,C79,C81,C82,C83)</f>
+      <c r="G90">
+        <f>AVERAGE(C76,C79,C80,C82,C83,C84)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I90" t="s">
         <v>13</v>
       </c>
-      <c r="J89">
+      <c r="J90">
         <v>3</v>
       </c>
-      <c r="K89">
-        <v>2</v>
-      </c>
-      <c r="M89" t="s">
+      <c r="K90">
+        <v>2</v>
+      </c>
+      <c r="M90" t="s">
         <v>13</v>
       </c>
-      <c r="N89">
-        <f>AVERAGE(B78,B81,B82,B83)</f>
+      <c r="N90">
+        <f>AVERAGE(B79,B82,B83,B84)</f>
         <v>1.5</v>
       </c>
-      <c r="O89">
-        <f>AVERAGE(C78,C81,C82,C83)</f>
+      <c r="O90">
+        <f>AVERAGE(C79,C82,C83,C84)</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E90" s="13" t="s">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E91" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F90" s="14" t="s">
+      <c r="F91" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G90" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I90" s="13" t="s">
+      <c r="G91" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I91" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J90" s="14" t="s">
+      <c r="J91" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K90" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M90" s="13" t="s">
+      <c r="K91" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M91" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N90" s="14" t="s">
+      <c r="N91" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O90" s="14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E91" s="12">
-        <v>1</v>
-      </c>
-      <c r="F91" s="11">
-        <f>MIN((($B$75-F88)^2+($C$75-G88)^2),(($B$75-F89)^2+($C$75-G89)^2))</f>
-        <v>8.8888888888888893</v>
-      </c>
-      <c r="G91" s="11">
-        <f>IF((($B$75-F88)^2+($C$75-G88)^2)&lt;(($B$75-F89)^2+($C$75-G89)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="I91" s="12">
-        <v>1</v>
-      </c>
-      <c r="J91" s="11">
-        <f>MIN((($B$75-J88)^2+($C$75-K88)^2),(($B$75-J89)^2+($C$75-K89)^2))</f>
-        <v>4</v>
-      </c>
-      <c r="K91" s="11">
-        <f>IF((($B$75-J88)^2+($C$75-K88)^2)&lt;(($B$75-J89)^2+($C$75-K89)^2),1,2)</f>
-        <v>1</v>
-      </c>
-      <c r="M91" s="12">
-        <v>1</v>
-      </c>
-      <c r="N91" s="11">
-        <f>MIN((($B$75-N88)^2+($C$75-O88)^2),(($B$75-N89)^2+($C$75-O89)^2))</f>
-        <v>6.3999999999999995</v>
-      </c>
-      <c r="O91" s="11">
-        <f>IF((($B$75-N88)^2+($C$75-O88)^2)&lt;(($B$75-N89)^2+($C$75-O89)^2),1,2)</f>
+      <c r="O91" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E92" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" s="11">
-        <f>MIN((($B$76-F88)^2+($C$76-G88)^2),(($B$76-F89)^2+($C$76-G89)^2))</f>
-        <v>2.2222222222222223</v>
+        <f>MIN((($B$76-F89)^2+($C$76-G89)^2),(($B$76-F90)^2+($C$76-G90)^2))</f>
+        <v>8.8888888888888893</v>
       </c>
       <c r="G92" s="11">
-        <f>IF((($B$76-F88)^2+($C$76-G88)^2)&lt;(($B$76-F89)^2+($C$76-G89)^2),1,2)</f>
-        <v>1</v>
+        <f>IF((($B$76-F89)^2+($C$76-G89)^2)&lt;(($B$76-F90)^2+($C$76-G90)^2),1,2)</f>
+        <v>2</v>
       </c>
       <c r="I92" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J92" s="11">
-        <f>MIN((($B$76-J88)^2+($C$76-K88)^2),(($B$76-J89)^2+($C$76-K89)^2))</f>
-        <v>5</v>
+        <f>MIN((($B$76-J89)^2+($C$76-K89)^2),(($B$76-J90)^2+($C$76-K90)^2))</f>
+        <v>4</v>
       </c>
       <c r="K92" s="11">
-        <f>IF((($B$76-J88)^2+($C$76-K88)^2)&lt;(($B$76-J89)^2+($C$76-K89)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$76-J89)^2+($C$76-K89)^2)&lt;(($B$76-J90)^2+($C$76-K90)^2),1,2)</f>
+        <v>1</v>
       </c>
       <c r="M92" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N92" s="11">
-        <f>MIN((($B$76-N88)^2+($C$76-O88)^2),(($B$76-N89)^2+($C$76-O89)^2))</f>
-        <v>0.7999999999999996</v>
+        <f>MIN((($B$76-N89)^2+($C$76-O89)^2),(($B$76-N90)^2+($C$76-O90)^2))</f>
+        <v>6.3999999999999995</v>
       </c>
       <c r="O92" s="11">
-        <f>IF((($B$76-N88)^2+($C$76-O88)^2)&lt;(($B$76-N89)^2+($C$76-O89)^2),1,2)</f>
+        <f>IF((($B$76-N89)^2+($C$76-O89)^2)&lt;(($B$76-N90)^2+($C$76-O90)^2),1,2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E93" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" s="11">
-        <f>MIN((($B$77-F88)^2+($C$77-G88)^2),(($B$77-F89)^2+($C$77-G89)^2))</f>
-        <v>0.88888888888888851</v>
+        <f>MIN((($B$77-F89)^2+($C$77-G89)^2),(($B$77-F90)^2+($C$77-G90)^2))</f>
+        <v>2.2222222222222223</v>
       </c>
       <c r="G93" s="11">
-        <f>IF((($B$77-F88)^2+($C$77-G88)^2)&lt;(($B$77-F89)^2+($C$77-G89)^2),1,2)</f>
+        <f>IF((($B$77-F89)^2+($C$77-G89)^2)&lt;(($B$77-F90)^2+($C$77-G90)^2),1,2)</f>
         <v>1</v>
       </c>
       <c r="I93" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J93" s="11">
-        <f>MIN((($B$77-J88)^2+($C$77-K88)^2),(($B$77-J89)^2+($C$77-K89)^2))</f>
+        <f>MIN((($B$77-J89)^2+($C$77-K89)^2),(($B$77-J90)^2+($C$77-K90)^2))</f>
         <v>5</v>
       </c>
       <c r="K93" s="11">
-        <f>IF((($B$77-J88)^2+($C$77-K88)^2)&lt;(($B$77-J89)^2+($C$77-K89)^2),1,2)</f>
+        <f>IF((($B$77-J89)^2+($C$77-K89)^2)&lt;(($B$77-J90)^2+($C$77-K90)^2),1,2)</f>
         <v>2</v>
       </c>
       <c r="M93" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N93" s="11">
-        <f>MIN((($B$77-N88)^2+($C$77-O88)^2),(($B$77-N89)^2+($C$77-O89)^2))</f>
-        <v>3.2</v>
+        <f>MIN((($B$77-N89)^2+($C$77-O89)^2),(($B$77-N90)^2+($C$77-O90)^2))</f>
+        <v>0.7999999999999996</v>
       </c>
       <c r="O93" s="11">
-        <f>IF((($B$77-N88)^2+($C$77-O88)^2)&lt;(($B$77-N89)^2+($C$77-O89)^2),1,2)</f>
+        <f>IF((($B$77-N89)^2+($C$77-O89)^2)&lt;(($B$77-N90)^2+($C$77-O90)^2),1,2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E94" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" s="11">
-        <f>MIN((($B$78-F88)^2+($C$78-G88)^2),(($B$78-F89)^2+($C$78-G89)^2))</f>
-        <v>2.2222222222222223</v>
+        <f>MIN((($B$78-F89)^2+($C$78-G89)^2),(($B$78-F90)^2+($C$78-G90)^2))</f>
+        <v>0.88888888888888851</v>
       </c>
       <c r="G94" s="11">
-        <f>IF((($B$78-F88)^2+($C$78-G88)^2)&lt;(($B$78-F89)^2+($C$78-G89)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$78-F89)^2+($C$78-G89)^2)&lt;(($B$78-F90)^2+($C$78-G90)^2),1,2)</f>
+        <v>1</v>
       </c>
       <c r="I94" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J94" s="11">
-        <f>MIN((($B$78-J88)^2+($C$78-K88)^2),(($B$78-J89)^2+($C$78-K89)^2))</f>
-        <v>0</v>
+        <f>MIN((($B$78-J89)^2+($C$78-K89)^2),(($B$78-J90)^2+($C$78-K90)^2))</f>
+        <v>5</v>
       </c>
       <c r="K94" s="11">
-        <f>IF((($B$78-J88)^2+($C$78-K88)^2)&lt;(($B$78-J89)^2+($C$78-K89)^2),1,2)</f>
-        <v>1</v>
+        <f>IF((($B$78-J89)^2+($C$78-K89)^2)&lt;(($B$78-J90)^2+($C$78-K90)^2),1,2)</f>
+        <v>2</v>
       </c>
       <c r="M94" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N94" s="11">
-        <f>MIN((($B$78-N88)^2+($C$78-O88)^2),(($B$78-N89)^2+($C$78-O89)^2))</f>
-        <v>4.5</v>
+        <f>MIN((($B$78-N89)^2+($C$78-O89)^2),(($B$78-N90)^2+($C$78-O90)^2))</f>
+        <v>3.2</v>
       </c>
       <c r="O94" s="11">
-        <f>IF((($B$78-N88)^2+($C$78-O88)^2)&lt;(($B$78-N89)^2+($C$78-O89)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$78-N89)^2+($C$78-O89)^2)&lt;(($B$78-N90)^2+($C$78-O90)^2),1,2)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E95" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" s="11">
-        <f>MIN((($B$79-F88)^2+($C$79-G88)^2),(($B$79-F89)^2+($C$79-G89)^2))</f>
-        <v>0.88888888888888906</v>
+        <f>MIN((($B$79-F89)^2+($C$79-G89)^2),(($B$79-F90)^2+($C$79-G90)^2))</f>
+        <v>2.2222222222222223</v>
       </c>
       <c r="G95" s="11">
-        <f>IF((($B$79-F88)^2+($C$79-G88)^2)&lt;(($B$79-F89)^2+($C$79-G89)^2),1,2)</f>
+        <f>IF((($B$79-F89)^2+($C$79-G89)^2)&lt;(($B$79-F90)^2+($C$79-G90)^2),1,2)</f>
         <v>2</v>
       </c>
       <c r="I95" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J95" s="11">
-        <f>MIN((($B$79-J88)^2+($C$79-K88)^2),(($B$79-J89)^2+($C$79-K89)^2))</f>
-        <v>1</v>
+        <f>MIN((($B$79-J89)^2+($C$79-K89)^2),(($B$79-J90)^2+($C$79-K90)^2))</f>
+        <v>0</v>
       </c>
       <c r="K95" s="11">
-        <f>IF((($B$79-J88)^2+($C$79-K88)^2)&lt;(($B$79-J89)^2+($C$79-K89)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$79-J89)^2+($C$79-K89)^2)&lt;(($B$79-J90)^2+($C$79-K90)^2),1,2)</f>
+        <v>1</v>
       </c>
       <c r="M95" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N95" s="11">
-        <f>MIN((($B$79-N88)^2+($C$79-O88)^2),(($B$79-N89)^2+($C$79-O89)^2))</f>
-        <v>1.6000000000000003</v>
+        <f>MIN((($B$79-N89)^2+($C$79-O89)^2),(($B$79-N90)^2+($C$79-O90)^2))</f>
+        <v>4.5</v>
       </c>
       <c r="O95" s="11">
-        <f>IF((($B$79-N88)^2+($C$79-O88)^2)&lt;(($B$79-N89)^2+($C$79-O89)^2),1,2)</f>
-        <v>1</v>
+        <f>IF((($B$79-N89)^2+($C$79-O89)^2)&lt;(($B$79-N90)^2+($C$79-O90)^2),1,2)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E96" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" s="11">
-        <f>MIN((($B$80-F88)^2+($C$80-G88)^2),(($B$80-F89)^2+($C$80-G89)^2))</f>
-        <v>2.2222222222222223</v>
+        <f>MIN((($B$80-F89)^2+($C$80-G89)^2),(($B$80-F90)^2+($C$80-G90)^2))</f>
+        <v>0.88888888888888906</v>
       </c>
       <c r="G96" s="11">
-        <f>IF((($B$80-F88)^2+($C$80-G88)^2)&lt;(($B$80-F89)^2+($C$80-G89)^2),1,2)</f>
-        <v>1</v>
+        <f>IF((($B$80-F89)^2+($C$80-G89)^2)&lt;(($B$80-F90)^2+($C$80-G90)^2),1,2)</f>
+        <v>2</v>
       </c>
       <c r="I96" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J96" s="11">
-        <f>MIN((($B$80-J88)^2+($C$80-K88)^2),(($B$80-J89)^2+($C$80-K89)^2))</f>
+        <f>MIN((($B$80-J89)^2+($C$80-K89)^2),(($B$80-J90)^2+($C$80-K90)^2))</f>
         <v>1</v>
       </c>
       <c r="K96" s="11">
-        <f>IF((($B$80-J88)^2+($C$80-K88)^2)&lt;(($B$80-J89)^2+($C$80-K89)^2),1,2)</f>
+        <f>IF((($B$80-J89)^2+($C$80-K89)^2)&lt;(($B$80-J90)^2+($C$80-K90)^2),1,2)</f>
         <v>2</v>
       </c>
       <c r="M96" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N96" s="11">
-        <f>MIN((($B$80-N88)^2+($C$80-O88)^2),(($B$80-N89)^2+($C$80-O89)^2))</f>
-        <v>4.0000000000000009</v>
+        <f>MIN((($B$80-N89)^2+($C$80-O89)^2),(($B$80-N90)^2+($C$80-O90)^2))</f>
+        <v>1.6000000000000003</v>
       </c>
       <c r="O96" s="11">
-        <f>IF((($B$80-N88)^2+($C$80-O88)^2)&lt;(($B$80-N89)^2+($C$80-O89)^2),1,2)</f>
+        <f>IF((($B$80-N89)^2+($C$80-O89)^2)&lt;(($B$80-N90)^2+($C$80-O90)^2),1,2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E97" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" s="11">
-        <f>MIN((($B$81-F88)^2+($C$81-G88)^2),(($B$81-F89)^2+($C$81-G89)^2))</f>
-        <v>3.5555555555555554</v>
+        <f>MIN((($B$81-F89)^2+($C$81-G89)^2),(($B$81-F90)^2+($C$81-G90)^2))</f>
+        <v>2.2222222222222223</v>
       </c>
       <c r="G97" s="11">
-        <f>IF((($B$81-F88)^2+($C$81-G88)^2)&lt;(($B$81-F89)^2+($C$81-G89)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$81-F89)^2+($C$81-G89)^2)&lt;(($B$81-F90)^2+($C$81-G90)^2),1,2)</f>
+        <v>1</v>
       </c>
       <c r="I97" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J97" s="11">
-        <f>MIN((($B$81-J88)^2+($C$81-K88)^2),(($B$81-J89)^2+($C$81-K89)^2))</f>
-        <v>4</v>
+        <f>MIN((($B$81-J89)^2+($C$81-K89)^2),(($B$81-J90)^2+($C$81-K90)^2))</f>
+        <v>1</v>
       </c>
       <c r="K97" s="11">
-        <f>IF((($B$81-J88)^2+($C$81-K88)^2)&lt;(($B$81-J89)^2+($C$81-K89)^2),1,2)</f>
-        <v>1</v>
+        <f>IF((($B$81-J89)^2+($C$81-K89)^2)&lt;(($B$81-J90)^2+($C$81-K90)^2),1,2)</f>
+        <v>2</v>
       </c>
       <c r="M97" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N97" s="11">
-        <f>MIN((($B$81-N88)^2+($C$81-O88)^2),(($B$81-N89)^2+($C$81-O89)^2))</f>
-        <v>2.5</v>
+        <f>MIN((($B$81-N89)^2+($C$81-O89)^2),(($B$81-N90)^2+($C$81-O90)^2))</f>
+        <v>4.0000000000000009</v>
       </c>
       <c r="O97" s="11">
-        <f>IF((($B$81-N88)^2+($C$81-O88)^2)&lt;(($B$81-N89)^2+($C$81-O89)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$81-N89)^2+($C$81-O89)^2)&lt;(($B$81-N90)^2+($C$81-O90)^2),1,2)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E98" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" s="11">
-        <f>MIN((($B$82-F88)^2+($C$82-G88)^2),(($B$82-F89)^2+($C$82-G89)^2))</f>
-        <v>2.2222222222222223</v>
+        <f>MIN((($B$82-F89)^2+($C$82-G89)^2),(($B$82-F90)^2+($C$82-G90)^2))</f>
+        <v>3.5555555555555554</v>
       </c>
       <c r="G98" s="11">
-        <f>IF((($B$82-F88)^2+($C$82-G88)^2)&lt;(($B$82-F89)^2+($C$82-G89)^2),1,2)</f>
+        <f>IF((($B$82-F89)^2+($C$82-G89)^2)&lt;(($B$82-F90)^2+($C$82-G90)^2),1,2)</f>
         <v>2</v>
       </c>
       <c r="I98" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J98" s="11">
-        <f>MIN((($B$82-J88)^2+($C$82-K88)^2),(($B$82-J89)^2+($C$82-K89)^2))</f>
-        <v>5</v>
+        <f>MIN((($B$82-J89)^2+($C$82-K89)^2),(($B$82-J90)^2+($C$82-K90)^2))</f>
+        <v>4</v>
       </c>
       <c r="K98" s="11">
-        <f>IF((($B$82-J88)^2+($C$82-K88)^2)&lt;(($B$82-J89)^2+($C$82-K89)^2),1,2)</f>
-        <v>2</v>
+        <f>IF((($B$82-J89)^2+($C$82-K89)^2)&lt;(($B$82-J90)^2+($C$82-K90)^2),1,2)</f>
+        <v>1</v>
       </c>
       <c r="M98" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N98" s="11">
-        <f>MIN((($B$82-N88)^2+($C$82-O88)^2),(($B$82-N89)^2+($C$82-O89)^2))</f>
-        <v>0.5</v>
+        <f>MIN((($B$82-N89)^2+($C$82-O89)^2),(($B$82-N90)^2+($C$82-O90)^2))</f>
+        <v>2.5</v>
       </c>
       <c r="O98" s="11">
-        <f>IF((($B$82-N88)^2+($C$82-O88)^2)&lt;(($B$82-N89)^2+($C$82-O89)^2),1,2)</f>
+        <f>IF((($B$82-N89)^2+($C$82-O89)^2)&lt;(($B$82-N90)^2+($C$82-O90)^2),1,2)</f>
         <v>2</v>
       </c>
     </row>
     <row r="99" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E99" s="12">
+        <v>8</v>
+      </c>
+      <c r="F99" s="11">
+        <f>MIN((($B$83-F89)^2+($C$83-G89)^2),(($B$83-F90)^2+($C$83-G90)^2))</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="G99" s="11">
+        <f>IF((($B$83-F89)^2+($C$83-G89)^2)&lt;(($B$83-F90)^2+($C$83-G90)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="I99" s="12">
+        <v>8</v>
+      </c>
+      <c r="J99" s="11">
+        <f>MIN((($B$83-J89)^2+($C$83-K89)^2),(($B$83-J90)^2+($C$83-K90)^2))</f>
+        <v>5</v>
+      </c>
+      <c r="K99" s="11">
+        <f>IF((($B$83-J89)^2+($C$83-K89)^2)&lt;(($B$83-J90)^2+($C$83-K90)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="M99" s="12">
+        <v>8</v>
+      </c>
+      <c r="N99" s="11">
+        <f>MIN((($B$83-N89)^2+($C$83-O89)^2),(($B$83-N90)^2+($C$83-O90)^2))</f>
+        <v>0.5</v>
+      </c>
+      <c r="O99" s="11">
+        <f>IF((($B$83-N89)^2+($C$83-O89)^2)&lt;(($B$83-N90)^2+($C$83-O90)^2),1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E100" s="12">
         <v>9</v>
       </c>
-      <c r="F99" s="11">
-        <f>MIN((($B$83-F88)^2+($C$83-G88)^2),(($B$83-F89)^2+($C$83-G89)^2))</f>
+      <c r="F100" s="11">
+        <f>MIN((($B$84-F89)^2+($C$84-G89)^2),(($B$84-F90)^2+($C$84-G90)^2))</f>
         <v>8.8888888888888893</v>
       </c>
-      <c r="G99" s="11">
-        <f>IF((($B$83-F88)^2+($C$83-G88)^2)&lt;(($B$83-F89)^2+($C$83-G89)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="I99" s="12">
+      <c r="G100" s="11">
+        <f>IF((($B$84-F89)^2+($C$84-G89)^2)&lt;(($B$84-F90)^2+($C$84-G90)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="I100" s="12">
         <v>9</v>
       </c>
-      <c r="J99" s="11">
-        <f>MIN((($B$83-J88)^2+($C$83-K88)^2),(($B$83-J89)^2+($C$83-K89)^2))</f>
-        <v>5</v>
-      </c>
-      <c r="K99" s="11">
-        <f>IF((($B$83-J88)^2+($C$83-K88)^2)&lt;(($B$83-J89)^2+($C$83-K89)^2),1,2)</f>
-        <v>2</v>
-      </c>
-      <c r="M99" s="12">
+      <c r="J100" s="11">
+        <f>MIN((($B$84-J89)^2+($C$84-K89)^2),(($B$84-J90)^2+($C$84-K90)^2))</f>
+        <v>5</v>
+      </c>
+      <c r="K100" s="11">
+        <f>IF((($B$84-J89)^2+($C$84-K89)^2)&lt;(($B$84-J90)^2+($C$84-K90)^2),1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="M100" s="12">
         <v>9</v>
       </c>
-      <c r="N99" s="11">
-        <f>MIN((($B$83-N88)^2+($C$83-O88)^2),(($B$83-N89)^2+($C$83-O89)^2))</f>
+      <c r="N100" s="11">
+        <f>MIN((($B$84-N89)^2+($C$84-O89)^2),(($B$84-N90)^2+($C$84-O90)^2))</f>
         <v>6.5</v>
       </c>
-      <c r="O99" s="11">
-        <f>IF((($B$83-N88)^2+($C$83-O88)^2)&lt;(($B$83-N89)^2+($C$83-O89)^2),1,2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E101" t="s">
-        <v>0</v>
-      </c>
-      <c r="F101" s="15">
-        <f>SUM(F91:F99)</f>
+      <c r="O100" s="11">
+        <f>IF((($B$84-N89)^2+($C$84-O89)^2)&lt;(($B$84-N90)^2+($C$84-O90)^2),1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>0</v>
+      </c>
+      <c r="F102" s="15">
+        <f>SUM(F92:F100)</f>
         <v>31.999999999999996</v>
       </c>
-      <c r="I101" t="s">
-        <v>0</v>
-      </c>
-      <c r="J101" s="15">
-        <f>SUM(J91:J99)</f>
+      <c r="I102" t="s">
+        <v>0</v>
+      </c>
+      <c r="J102" s="15">
+        <f>SUM(J92:J100)</f>
         <v>30</v>
       </c>
-      <c r="M101" t="s">
-        <v>0</v>
-      </c>
-      <c r="N101" s="15">
-        <f>SUM(N91:N99)</f>
+      <c r="M102" t="s">
+        <v>0</v>
+      </c>
+      <c r="N102" s="15">
+        <f>SUM(N92:N100)</f>
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="I71:K71"/>
-    <mergeCell ref="M71:O71"/>
-    <mergeCell ref="I87:K87"/>
-    <mergeCell ref="M87:O87"/>
-    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="M72:O72"/>
+    <mergeCell ref="I88:K88"/>
+    <mergeCell ref="M88:O88"/>
+    <mergeCell ref="E88:G88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>